<commit_message>
6502 CPU initial structure with microcode
</commit_message>
<xml_diff>
--- a/cpu/opcodes.xlsx
+++ b/cpu/opcodes.xlsx
@@ -1,18 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18067"/>
+  <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zhiyb\Documents\Design\FPGA\CPU_demo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zhiyb\Documents\Design\FPGA\SVNES\cpu\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9510"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Opcode" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="69">
   <si>
     <t>Imp</t>
   </si>
@@ -237,7 +237,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -246,24 +246,29 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color theme="8"/>
+      <color rgb="FF9C5700"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <i/>
       <sz val="11"/>
-      <color theme="5"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -272,8 +277,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
   </fills>
@@ -295,35 +304,24 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Good" xfId="2" builtinId="26"/>
+    <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -355,7 +353,13 @@
       <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
           <xdr14:nvContentPartPr>
-            <xdr14:cNvPr id="6" name="Ink 5"/>
+            <xdr14:cNvPr id="6" name="Ink 5">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006000000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
             <xdr14:cNvContentPartPr/>
           </xdr14:nvContentPartPr>
           <xdr14:nvPr macro=""/>
@@ -693,47 +697,46 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA35"/>
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="A1:Z35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="S22" sqref="S22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="3.875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="3.625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="4.625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="4.375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="4.25" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="3.75" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="4.75" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="4.625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="3.375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="2.875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="4.25" customWidth="1"/>
-    <col min="15" max="15" width="4.375" style="3" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="3.875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="4.375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="3.625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="4.625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="4.5" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="3.75" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="4.75" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="4.625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="3.375" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="4.375" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="4.25" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="2.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="3.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="3.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="3.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="4.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="4.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="3.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="2.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="4.28515625" customWidth="1"/>
+    <col min="15" max="15" width="4.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="3.85546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="3.5703125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="3.7109375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="4.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="4.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="3.42578125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="4.28515625" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>60</v>
       </c>
@@ -761,19 +764,19 @@
       <c r="I1" t="s">
         <v>2</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="2" t="s">
         <v>65</v>
       </c>
       <c r="L1" t="s">
         <v>3</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="O1" s="1" t="s">
         <v>60</v>
       </c>
       <c r="P1" t="s">
@@ -794,10 +797,10 @@
       <c r="U1" t="s">
         <v>2</v>
       </c>
-      <c r="V1" t="s">
+      <c r="V1" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="W1" t="s">
+      <c r="W1" s="2" t="s">
         <v>65</v>
       </c>
       <c r="X1" t="s">
@@ -806,14 +809,11 @@
       <c r="Y1" t="s">
         <v>66</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="Z1" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="AA1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -823,25 +823,25 @@
       <c r="D2">
         <v>3</v>
       </c>
-      <c r="E2" s="4">
-        <v>4</v>
-      </c>
-      <c r="G2" s="4">
-        <v>6</v>
-      </c>
-      <c r="H2" s="1">
+      <c r="E2">
+        <v>4</v>
+      </c>
+      <c r="G2">
+        <v>6</v>
+      </c>
+      <c r="H2">
         <v>5</v>
       </c>
       <c r="I2">
         <v>4</v>
       </c>
-      <c r="J2" s="1">
-        <v>4</v>
-      </c>
-      <c r="K2" s="1">
-        <v>4</v>
-      </c>
-      <c r="O2" s="3" t="s">
+      <c r="J2" s="3">
+        <v>4</v>
+      </c>
+      <c r="K2" s="3">
+        <v>4</v>
+      </c>
+      <c r="O2" s="1" t="s">
         <v>31</v>
       </c>
       <c r="U2">
@@ -851,7 +851,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -861,32 +861,32 @@
       <c r="D3">
         <v>3</v>
       </c>
-      <c r="E3" s="4">
-        <v>4</v>
-      </c>
-      <c r="G3" s="4">
-        <v>6</v>
-      </c>
-      <c r="H3" s="1">
+      <c r="E3">
+        <v>4</v>
+      </c>
+      <c r="G3">
+        <v>6</v>
+      </c>
+      <c r="H3">
         <v>5</v>
       </c>
       <c r="I3">
         <v>4</v>
       </c>
-      <c r="J3" s="1">
-        <v>4</v>
-      </c>
-      <c r="K3" s="1">
-        <v>4</v>
-      </c>
-      <c r="O3" s="3" t="s">
+      <c r="J3" s="3">
+        <v>4</v>
+      </c>
+      <c r="K3" s="3">
+        <v>4</v>
+      </c>
+      <c r="O3" s="1" t="s">
         <v>32</v>
       </c>
       <c r="U3">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -896,32 +896,32 @@
       <c r="D4">
         <v>3</v>
       </c>
-      <c r="E4" s="4">
-        <v>4</v>
-      </c>
-      <c r="G4" s="4">
-        <v>6</v>
-      </c>
-      <c r="H4" s="1">
+      <c r="E4">
+        <v>4</v>
+      </c>
+      <c r="G4">
+        <v>6</v>
+      </c>
+      <c r="H4">
         <v>5</v>
       </c>
       <c r="I4">
         <v>4</v>
       </c>
-      <c r="J4" s="1">
-        <v>4</v>
-      </c>
-      <c r="K4" s="1">
-        <v>4</v>
-      </c>
-      <c r="O4" s="3" t="s">
+      <c r="J4" s="3">
+        <v>4</v>
+      </c>
+      <c r="K4" s="3">
+        <v>4</v>
+      </c>
+      <c r="O4" s="1" t="s">
         <v>33</v>
       </c>
       <c r="P4">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -931,32 +931,32 @@
       <c r="D5">
         <v>3</v>
       </c>
-      <c r="E5" s="4">
-        <v>4</v>
-      </c>
-      <c r="G5" s="4">
-        <v>6</v>
-      </c>
-      <c r="H5" s="1">
+      <c r="E5">
+        <v>4</v>
+      </c>
+      <c r="G5">
+        <v>6</v>
+      </c>
+      <c r="H5">
         <v>5</v>
       </c>
       <c r="I5">
         <v>4</v>
       </c>
-      <c r="J5" s="1">
-        <v>4</v>
-      </c>
-      <c r="K5" s="1">
-        <v>4</v>
-      </c>
-      <c r="O5" s="3" t="s">
+      <c r="J5" s="3">
+        <v>4</v>
+      </c>
+      <c r="K5" s="3">
+        <v>4</v>
+      </c>
+      <c r="O5" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="P5" s="4">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="P5">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -966,169 +966,169 @@
       <c r="D6">
         <v>3</v>
       </c>
-      <c r="E6" s="4">
-        <v>4</v>
-      </c>
-      <c r="G6" s="4">
-        <v>6</v>
-      </c>
-      <c r="H6" s="1">
+      <c r="E6">
+        <v>4</v>
+      </c>
+      <c r="G6">
+        <v>6</v>
+      </c>
+      <c r="H6">
         <v>5</v>
       </c>
       <c r="I6">
         <v>4</v>
       </c>
-      <c r="J6" s="1">
-        <v>4</v>
-      </c>
-      <c r="K6" s="1">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="O7" s="3" t="s">
+      <c r="J6" s="3">
+        <v>4</v>
+      </c>
+      <c r="K6" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="O7" s="1" t="s">
         <v>35</v>
       </c>
       <c r="P7">
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>9</v>
       </c>
       <c r="B8">
         <v>2</v>
       </c>
-      <c r="D8" s="4">
-        <v>5</v>
-      </c>
-      <c r="E8" s="4">
-        <v>6</v>
-      </c>
-      <c r="I8" s="4">
-        <v>6</v>
-      </c>
-      <c r="J8" s="4">
+      <c r="D8">
+        <v>5</v>
+      </c>
+      <c r="E8">
+        <v>6</v>
+      </c>
+      <c r="I8">
+        <v>6</v>
+      </c>
+      <c r="J8" s="3">
         <v>7</v>
       </c>
-      <c r="O8" s="3" t="s">
+      <c r="O8" s="1" t="s">
         <v>36</v>
       </c>
       <c r="P8">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>10</v>
       </c>
       <c r="B9">
         <v>2</v>
       </c>
-      <c r="D9" s="4">
-        <v>5</v>
-      </c>
-      <c r="E9" s="4">
-        <v>6</v>
-      </c>
-      <c r="I9" s="4">
-        <v>6</v>
-      </c>
-      <c r="J9" s="4">
+      <c r="D9">
+        <v>5</v>
+      </c>
+      <c r="E9">
+        <v>6</v>
+      </c>
+      <c r="I9">
+        <v>6</v>
+      </c>
+      <c r="J9" s="3">
         <v>7</v>
       </c>
-      <c r="O9" s="3" t="s">
+      <c r="O9" s="1" t="s">
         <v>37</v>
       </c>
       <c r="P9">
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>11</v>
       </c>
       <c r="B10">
         <v>2</v>
       </c>
-      <c r="D10" s="4">
-        <v>5</v>
-      </c>
-      <c r="E10" s="4">
-        <v>6</v>
-      </c>
-      <c r="I10" s="4">
-        <v>6</v>
-      </c>
-      <c r="J10" s="4">
+      <c r="D10">
+        <v>5</v>
+      </c>
+      <c r="E10">
+        <v>6</v>
+      </c>
+      <c r="I10">
+        <v>6</v>
+      </c>
+      <c r="J10" s="3">
         <v>7</v>
       </c>
-      <c r="O10" s="3" t="s">
+      <c r="O10" s="1" t="s">
         <v>38</v>
       </c>
       <c r="P10">
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>12</v>
       </c>
       <c r="B11">
         <v>2</v>
       </c>
-      <c r="D11" s="4">
-        <v>5</v>
-      </c>
-      <c r="E11" s="4">
-        <v>6</v>
-      </c>
-      <c r="I11" s="4">
-        <v>6</v>
-      </c>
-      <c r="J11" s="4">
+      <c r="D11">
+        <v>5</v>
+      </c>
+      <c r="E11">
+        <v>6</v>
+      </c>
+      <c r="I11">
+        <v>6</v>
+      </c>
+      <c r="J11" s="3">
         <v>7</v>
       </c>
-      <c r="O11" s="3" t="s">
+      <c r="O11" s="1" t="s">
         <v>39</v>
       </c>
       <c r="P11">
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="O12" s="3" t="s">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="O12" s="1" t="s">
         <v>40</v>
       </c>
       <c r="P12">
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>13</v>
       </c>
-      <c r="D13" s="4">
-        <v>5</v>
-      </c>
-      <c r="E13" s="4">
-        <v>6</v>
-      </c>
-      <c r="I13" s="4">
-        <v>6</v>
-      </c>
-      <c r="J13" s="4">
+      <c r="D13">
+        <v>5</v>
+      </c>
+      <c r="E13">
+        <v>6</v>
+      </c>
+      <c r="I13">
+        <v>6</v>
+      </c>
+      <c r="J13" s="3">
         <v>7</v>
       </c>
-      <c r="O13" s="3" t="s">
+      <c r="O13" s="1" t="s">
         <v>41</v>
       </c>
       <c r="P13">
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -1136,37 +1136,37 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>15</v>
       </c>
       <c r="B15">
         <v>2</v>
       </c>
-      <c r="O15" s="3" t="s">
+      <c r="O15" s="1" t="s">
         <v>42</v>
       </c>
       <c r="P15">
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>16</v>
       </c>
-      <c r="D16" s="4">
-        <v>5</v>
-      </c>
-      <c r="E16" s="4">
-        <v>6</v>
-      </c>
-      <c r="I16" s="4">
-        <v>6</v>
-      </c>
-      <c r="J16" s="4">
+      <c r="D16">
+        <v>5</v>
+      </c>
+      <c r="E16">
+        <v>6</v>
+      </c>
+      <c r="I16">
+        <v>6</v>
+      </c>
+      <c r="J16" s="3">
         <v>7</v>
       </c>
-      <c r="O16" s="3" t="s">
+      <c r="O16" s="1" t="s">
         <v>43</v>
       </c>
       <c r="P16">
@@ -1180,7 +1180,7 @@
       <c r="B17">
         <v>2</v>
       </c>
-      <c r="O17" s="3" t="s">
+      <c r="O17" s="1" t="s">
         <v>44</v>
       </c>
       <c r="P17">
@@ -1194,7 +1194,7 @@
       <c r="B18">
         <v>2</v>
       </c>
-      <c r="O18" s="3" t="s">
+      <c r="O18" s="1" t="s">
         <v>45</v>
       </c>
       <c r="P18">
@@ -1202,7 +1202,7 @@
       </c>
     </row>
     <row r="19" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="O19" s="3" t="s">
+      <c r="O19" s="1" t="s">
         <v>46</v>
       </c>
       <c r="P19">
@@ -1219,7 +1219,7 @@
       <c r="I20">
         <v>4</v>
       </c>
-      <c r="O20" s="3" t="s">
+      <c r="O20" s="1" t="s">
         <v>47</v>
       </c>
       <c r="P20">
@@ -1236,22 +1236,22 @@
       <c r="D21">
         <v>3</v>
       </c>
-      <c r="E21" s="4">
-        <v>4</v>
-      </c>
-      <c r="G21" s="4">
-        <v>6</v>
-      </c>
-      <c r="H21" s="1">
+      <c r="E21">
+        <v>4</v>
+      </c>
+      <c r="G21">
+        <v>6</v>
+      </c>
+      <c r="H21">
         <v>5</v>
       </c>
       <c r="I21">
         <v>4</v>
       </c>
-      <c r="J21" s="1">
-        <v>4</v>
-      </c>
-      <c r="K21" s="1">
+      <c r="J21" s="3">
+        <v>4</v>
+      </c>
+      <c r="K21" s="3">
         <v>4</v>
       </c>
     </row>
@@ -1268,31 +1268,31 @@
       <c r="I22">
         <v>4</v>
       </c>
-      <c r="O22" s="3" t="s">
+      <c r="O22" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="Q22">
-        <v>2</v>
-      </c>
-      <c r="R22">
-        <v>3</v>
-      </c>
-      <c r="S22" s="4">
+      <c r="Q22" s="4">
+        <v>2</v>
+      </c>
+      <c r="R22" s="4">
+        <v>3</v>
+      </c>
+      <c r="S22">
         <v>4</v>
       </c>
       <c r="U22">
         <v>4</v>
       </c>
-      <c r="V22" s="1">
-        <v>4</v>
-      </c>
-      <c r="W22" s="1">
-        <v>4</v>
-      </c>
-      <c r="Y22" s="4">
-        <v>6</v>
-      </c>
-      <c r="Z22" s="1">
+      <c r="V22" s="3">
+        <v>4</v>
+      </c>
+      <c r="W22" s="3">
+        <v>4</v>
+      </c>
+      <c r="Y22">
+        <v>6</v>
+      </c>
+      <c r="Z22" s="3">
         <v>5</v>
       </c>
     </row>
@@ -1309,42 +1309,42 @@
       <c r="I23">
         <v>4</v>
       </c>
-      <c r="O23" s="3" t="s">
+      <c r="O23" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="Q23">
-        <v>2</v>
-      </c>
-      <c r="R23">
-        <v>3</v>
-      </c>
-      <c r="T23" s="4">
+      <c r="Q23" s="4">
+        <v>2</v>
+      </c>
+      <c r="R23" s="4">
+        <v>3</v>
+      </c>
+      <c r="T23">
         <v>4</v>
       </c>
       <c r="U23">
         <v>4</v>
       </c>
-      <c r="W23" s="1">
+      <c r="W23" s="3">
         <v>4</v>
       </c>
     </row>
     <row r="24" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="O24" s="3" t="s">
+      <c r="O24" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="Q24">
-        <v>2</v>
-      </c>
-      <c r="R24">
-        <v>3</v>
-      </c>
-      <c r="S24" s="4">
+      <c r="Q24" s="4">
+        <v>2</v>
+      </c>
+      <c r="R24" s="4">
+        <v>3</v>
+      </c>
+      <c r="S24">
         <v>4</v>
       </c>
       <c r="U24">
         <v>4</v>
       </c>
-      <c r="V24" s="1">
+      <c r="V24" s="3">
         <v>4</v>
       </c>
     </row>
@@ -1352,31 +1352,31 @@
       <c r="A25" t="s">
         <v>23</v>
       </c>
-      <c r="M25" s="2">
-        <v>2</v>
-      </c>
-      <c r="O25" s="3" t="s">
+      <c r="M25" s="3">
+        <v>2</v>
+      </c>
+      <c r="O25" s="1" t="s">
         <v>51</v>
       </c>
       <c r="R25">
         <v>3</v>
       </c>
-      <c r="S25" s="4">
+      <c r="S25">
         <v>4</v>
       </c>
       <c r="U25">
         <v>4</v>
       </c>
-      <c r="V25" s="4">
-        <v>5</v>
-      </c>
-      <c r="W25" s="4">
-        <v>5</v>
-      </c>
-      <c r="Y25" s="4">
-        <v>6</v>
-      </c>
-      <c r="Z25" s="4">
+      <c r="V25" s="3">
+        <v>5</v>
+      </c>
+      <c r="W25" s="3">
+        <v>5</v>
+      </c>
+      <c r="Y25">
+        <v>6</v>
+      </c>
+      <c r="Z25" s="3">
         <v>6</v>
       </c>
     </row>
@@ -1384,16 +1384,16 @@
       <c r="A26" t="s">
         <v>24</v>
       </c>
-      <c r="M26" s="2">
-        <v>2</v>
-      </c>
-      <c r="O26" s="3" t="s">
+      <c r="M26" s="3">
+        <v>2</v>
+      </c>
+      <c r="O26" s="1" t="s">
         <v>52</v>
       </c>
       <c r="R26">
         <v>3</v>
       </c>
-      <c r="T26" s="4">
+      <c r="T26">
         <v>4</v>
       </c>
       <c r="U26">
@@ -1404,16 +1404,16 @@
       <c r="A27" t="s">
         <v>25</v>
       </c>
-      <c r="M27" s="2">
-        <v>2</v>
-      </c>
-      <c r="O27" s="3" t="s">
+      <c r="M27" s="3">
+        <v>2</v>
+      </c>
+      <c r="O27" s="1" t="s">
         <v>53</v>
       </c>
       <c r="R27">
         <v>3</v>
       </c>
-      <c r="S27" s="4">
+      <c r="S27">
         <v>4</v>
       </c>
       <c r="U27">
@@ -1424,7 +1424,7 @@
       <c r="A28" t="s">
         <v>26</v>
       </c>
-      <c r="M28" s="2">
+      <c r="M28" s="3">
         <v>2</v>
       </c>
     </row>
@@ -1432,10 +1432,10 @@
       <c r="A29" t="s">
         <v>27</v>
       </c>
-      <c r="M29" s="2">
-        <v>2</v>
-      </c>
-      <c r="O29" s="3" t="s">
+      <c r="M29" s="3">
+        <v>2</v>
+      </c>
+      <c r="O29" s="1" t="s">
         <v>54</v>
       </c>
       <c r="P29">
@@ -1446,10 +1446,10 @@
       <c r="A30" t="s">
         <v>28</v>
       </c>
-      <c r="M30" s="2">
-        <v>2</v>
-      </c>
-      <c r="O30" s="3" t="s">
+      <c r="M30" s="3">
+        <v>2</v>
+      </c>
+      <c r="O30" s="1" t="s">
         <v>55</v>
       </c>
       <c r="P30">
@@ -1460,10 +1460,10 @@
       <c r="A31" t="s">
         <v>29</v>
       </c>
-      <c r="M31" s="2">
-        <v>2</v>
-      </c>
-      <c r="O31" s="3" t="s">
+      <c r="M31" s="3">
+        <v>2</v>
+      </c>
+      <c r="O31" s="1" t="s">
         <v>56</v>
       </c>
       <c r="P31">
@@ -1474,10 +1474,10 @@
       <c r="A32" t="s">
         <v>30</v>
       </c>
-      <c r="M32" s="2">
-        <v>2</v>
-      </c>
-      <c r="O32" s="3" t="s">
+      <c r="M32" s="3">
+        <v>2</v>
+      </c>
+      <c r="O32" s="1" t="s">
         <v>57</v>
       </c>
       <c r="P32">
@@ -1485,7 +1485,7 @@
       </c>
     </row>
     <row r="34" spans="15:16" x14ac:dyDescent="0.25">
-      <c r="O34" s="3" t="s">
+      <c r="O34" s="1" t="s">
         <v>58</v>
       </c>
       <c r="P34">
@@ -1493,7 +1493,7 @@
       </c>
     </row>
     <row r="35" spans="15:16" x14ac:dyDescent="0.25">
-      <c r="O35" s="3" t="s">
+      <c r="O35" s="1" t="s">
         <v>59</v>
       </c>
       <c r="P35">
@@ -1501,11 +1501,6 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="Q15:XFD20 O21:XFD21 B2:B6 O14:XFD14 Q7:XFD13 O28:XFD28 C8:C11 B16:C16 C17:F18 V2:W2 O36:XFD1048576 A19:F19 L2:L6 F2:F6 J20:L20 A24:L24 M2:M24 A7:L7 S23 B20:C20 E20:H20 O33:XFD33 Q29:XFD32 B21:B23 B25:L32 A33:M1048576 A12:L12 F8:H11 K8:L11 B13:C13 C14:L15 F13:H13 K13:L13 G17:L19 K16:L16 F16:H16 T27 S26 T24:T25 T22 E22:H23 F21 V26:XFD27 W24:XFD24 V23 X23:XFD23 X25 J22:L23 L21 P25:Q27 P22:P24 X22 AA22:XFD22 AA25:XFD25 Y2:XFD2 P2:T3 V3:XFD3 O6:XFD6 Q4:XFD5 Q34:XFD35">
-    <cfRule type="notContainsBlanks" dxfId="1" priority="1">
-      <formula>LEN(TRIM(A2))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>

</xml_diff>

<commit_message>
Load indexed zero page access
</commit_message>
<xml_diff>
--- a/cpu/opcodes.xlsx
+++ b/cpu/opcodes.xlsx
@@ -704,7 +704,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="S22" sqref="S22"/>
+      <selection pane="bottomRight" activeCell="U22" sqref="U22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1277,7 +1277,7 @@
       <c r="R22" s="4">
         <v>3</v>
       </c>
-      <c r="S22">
+      <c r="S22" s="4">
         <v>4</v>
       </c>
       <c r="U22">
@@ -1318,7 +1318,7 @@
       <c r="R23" s="4">
         <v>3</v>
       </c>
-      <c r="T23">
+      <c r="T23" s="4">
         <v>4</v>
       </c>
       <c r="U23">
@@ -1338,7 +1338,7 @@
       <c r="R24" s="4">
         <v>3</v>
       </c>
-      <c r="S24">
+      <c r="S24" s="4">
         <v>4</v>
       </c>
       <c r="U24">

</xml_diff>

<commit_message>
Load indexed absolute addressing
</commit_message>
<xml_diff>
--- a/cpu/opcodes.xlsx
+++ b/cpu/opcodes.xlsx
@@ -237,7 +237,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -260,13 +260,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -282,7 +275,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -304,20 +298,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="3">
-    <cellStyle name="Good" xfId="2" builtinId="26"/>
+  <cellStyles count="2">
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -704,7 +697,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="V22" sqref="V22"/>
+      <selection pane="bottomRight" activeCell="Y22" sqref="Y22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1283,10 +1276,10 @@
       <c r="U22" s="4">
         <v>4</v>
       </c>
-      <c r="V22" s="3">
-        <v>4</v>
-      </c>
-      <c r="W22" s="3">
+      <c r="V22" s="5">
+        <v>4</v>
+      </c>
+      <c r="W22" s="5">
         <v>4</v>
       </c>
       <c r="Y22">
@@ -1324,7 +1317,7 @@
       <c r="U23" s="4">
         <v>4</v>
       </c>
-      <c r="W23" s="3">
+      <c r="W23" s="5">
         <v>4</v>
       </c>
     </row>
@@ -1344,7 +1337,7 @@
       <c r="U24" s="4">
         <v>4</v>
       </c>
-      <c r="V24" s="3">
+      <c r="V24" s="5">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Load post-indexed indirect addressing
</commit_message>
<xml_diff>
--- a/cpu/opcodes.xlsx
+++ b/cpu/opcodes.xlsx
@@ -697,7 +697,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="Y22" sqref="Y22"/>
+      <selection pane="bottomRight" activeCell="R25" sqref="R25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1282,10 +1282,10 @@
       <c r="W22" s="5">
         <v>4</v>
       </c>
-      <c r="Y22">
-        <v>6</v>
-      </c>
-      <c r="Z22" s="3">
+      <c r="Y22" s="4">
+        <v>6</v>
+      </c>
+      <c r="Z22" s="5">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Store zero page addressing
</commit_message>
<xml_diff>
--- a/cpu/opcodes.xlsx
+++ b/cpu/opcodes.xlsx
@@ -302,13 +302,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
@@ -694,10 +695,10 @@
   <dimension ref="A1:Z35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="R25" sqref="R25"/>
+      <selection pane="bottomRight" activeCell="S25" sqref="S25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1351,7 +1352,7 @@
       <c r="O25" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="R25">
+      <c r="R25" s="4">
         <v>3</v>
       </c>
       <c r="S25">
@@ -1360,16 +1361,17 @@
       <c r="U25">
         <v>4</v>
       </c>
-      <c r="V25" s="3">
-        <v>5</v>
-      </c>
-      <c r="W25" s="3">
-        <v>5</v>
-      </c>
-      <c r="Y25">
-        <v>6</v>
-      </c>
-      <c r="Z25" s="3">
+      <c r="V25" s="6">
+        <v>5</v>
+      </c>
+      <c r="W25" s="6">
+        <v>5</v>
+      </c>
+      <c r="X25" s="6"/>
+      <c r="Y25" s="6">
+        <v>6</v>
+      </c>
+      <c r="Z25" s="6">
         <v>6</v>
       </c>
     </row>
@@ -1383,7 +1385,7 @@
       <c r="O26" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="R26">
+      <c r="R26" s="4">
         <v>3</v>
       </c>
       <c r="T26">
@@ -1403,7 +1405,7 @@
       <c r="O27" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="R27">
+      <c r="R27" s="4">
         <v>3</v>
       </c>
       <c r="S27">

</xml_diff>

<commit_message>
Store indexed zero page addressing
</commit_message>
<xml_diff>
--- a/cpu/opcodes.xlsx
+++ b/cpu/opcodes.xlsx
@@ -698,7 +698,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="S25" sqref="S25"/>
+      <selection pane="bottomRight" activeCell="U25" sqref="U25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1355,7 +1355,7 @@
       <c r="R25" s="4">
         <v>3</v>
       </c>
-      <c r="S25">
+      <c r="S25" s="4">
         <v>4</v>
       </c>
       <c r="U25">
@@ -1388,7 +1388,7 @@
       <c r="R26" s="4">
         <v>3</v>
       </c>
-      <c r="T26">
+      <c r="T26" s="4">
         <v>4</v>
       </c>
       <c r="U26">
@@ -1408,7 +1408,7 @@
       <c r="R27" s="4">
         <v>3</v>
       </c>
-      <c r="S27">
+      <c r="S27" s="4">
         <v>4</v>
       </c>
       <c r="U27">

</xml_diff>

<commit_message>
Store indexed absolute addressing
</commit_message>
<xml_diff>
--- a/cpu/opcodes.xlsx
+++ b/cpu/opcodes.xlsx
@@ -302,7 +302,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
@@ -310,6 +310,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
@@ -698,7 +699,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="V25" sqref="V25"/>
+      <selection pane="bottomRight" activeCell="Y25" sqref="Y25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1361,10 +1362,10 @@
       <c r="U25" s="4">
         <v>4</v>
       </c>
-      <c r="V25" s="6">
-        <v>5</v>
-      </c>
-      <c r="W25" s="6">
+      <c r="V25" s="7">
+        <v>5</v>
+      </c>
+      <c r="W25" s="7">
         <v>5</v>
       </c>
       <c r="X25" s="6"/>

</xml_diff>

<commit_message>
AND #i, ORA #i, EOR #i
</commit_message>
<xml_diff>
--- a/cpu/opcodes.xlsx
+++ b/cpu/opcodes.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18067"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18528"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9510"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9510" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Opcode" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="171027"/>
+  <fileRecoveryPr autoRecover="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -236,8 +237,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -260,8 +261,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -277,6 +291,11 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
   </fills>
@@ -298,11 +317,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
@@ -311,8 +331,10 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Good" xfId="2" builtinId="26"/>
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -691,7 +713,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:Z35"/>
   <sheetViews>
@@ -699,7 +721,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="U2" sqref="U2"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -812,7 +834,7 @@
       <c r="A2" t="s">
         <v>4</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="8">
         <v>2</v>
       </c>
       <c r="D2">
@@ -850,7 +872,7 @@
       <c r="A3" t="s">
         <v>5</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="8">
         <v>2</v>
       </c>
       <c r="D3">
@@ -885,7 +907,7 @@
       <c r="A4" t="s">
         <v>6</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="4">
         <v>2</v>
       </c>
       <c r="D4">
@@ -920,7 +942,7 @@
       <c r="A5" t="s">
         <v>7</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="4">
         <v>2</v>
       </c>
       <c r="D5">
@@ -955,7 +977,7 @@
       <c r="A6" t="s">
         <v>8</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="4">
         <v>2</v>
       </c>
       <c r="D6">

</xml_diff>

<commit_message>
ADC d, SBC d, AND d, ORA d, EOR d
</commit_message>
<xml_diff>
--- a/cpu/opcodes.xlsx
+++ b/cpu/opcodes.xlsx
@@ -837,7 +837,7 @@
       <c r="C2" s="8">
         <v>2</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="4">
         <v>3</v>
       </c>
       <c r="E2">
@@ -875,7 +875,7 @@
       <c r="C3" s="8">
         <v>2</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="4">
         <v>3</v>
       </c>
       <c r="E3">
@@ -910,7 +910,7 @@
       <c r="C4" s="4">
         <v>2</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="4">
         <v>3</v>
       </c>
       <c r="E4">
@@ -945,7 +945,7 @@
       <c r="C5" s="4">
         <v>2</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="4">
         <v>3</v>
       </c>
       <c r="E5">
@@ -980,7 +980,7 @@
       <c r="C6" s="4">
         <v>2</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="4">
         <v>3</v>
       </c>
       <c r="E6">

</xml_diff>

<commit_message>
d, x: ADC, SBC, AND, ORA, EOR
</commit_message>
<xml_diff>
--- a/cpu/opcodes.xlsx
+++ b/cpu/opcodes.xlsx
@@ -840,7 +840,7 @@
       <c r="D2" s="4">
         <v>3</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="4">
         <v>4</v>
       </c>
       <c r="G2">
@@ -878,7 +878,7 @@
       <c r="D3" s="4">
         <v>3</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="4">
         <v>4</v>
       </c>
       <c r="G3">
@@ -913,7 +913,7 @@
       <c r="D4" s="4">
         <v>3</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="4">
         <v>4</v>
       </c>
       <c r="G4">
@@ -948,7 +948,7 @@
       <c r="D5" s="4">
         <v>3</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="4">
         <v>4</v>
       </c>
       <c r="G5">
@@ -983,7 +983,7 @@
       <c r="D6" s="4">
         <v>3</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="4">
         <v>4</v>
       </c>
       <c r="G6">

</xml_diff>

<commit_message>
LDA now uses the same microcode branch as arithmetic ops
</commit_message>
<xml_diff>
--- a/cpu/opcodes.xlsx
+++ b/cpu/opcodes.xlsx
@@ -322,16 +322,18 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Good" xfId="2" builtinId="26"/>
@@ -734,23 +736,22 @@
     <col min="6" max="7" width="4.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="4.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="3.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="4.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="4.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="4.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="4.5703125" style="2" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="3.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="2.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="2.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="4.28515625" customWidth="1"/>
     <col min="15" max="15" width="4.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="3.85546875" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="4.42578125" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="3.5703125" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="4.5703125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="4.42578125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="3.7109375" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="4.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="4.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="3.42578125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="4.42578125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="4.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="20" max="21" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="4.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="3.7109375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="4.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="4.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="3.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.25">
@@ -775,72 +776,73 @@
       <c r="G1" t="s">
         <v>66</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="I1" t="s">
-        <v>2</v>
-      </c>
-      <c r="J1" s="2" t="s">
+      <c r="I1" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="J1" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="L1" t="s">
-        <v>3</v>
-      </c>
-      <c r="M1" s="2" t="s">
+      <c r="L1" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="M1" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="N1" s="9"/>
+      <c r="O1" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="P1" t="s">
+      <c r="P1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="Q1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="R1" t="s">
+      <c r="R1" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="S1" t="s">
+      <c r="S1" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="T1" t="s">
+      <c r="T1" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="U1" t="s">
-        <v>2</v>
-      </c>
-      <c r="V1" s="2" t="s">
+      <c r="U1" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="V1" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="W1" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="X1" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="W1" s="2" t="s">
+      <c r="Y1" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="X1" t="s">
-        <v>3</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>66</v>
-      </c>
-      <c r="Z1" s="2" t="s">
-        <v>67</v>
+      <c r="Z1" s="9" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="8">
-        <v>2</v>
-      </c>
-      <c r="D2" s="4">
-        <v>3</v>
-      </c>
-      <c r="E2" s="4">
+      <c r="C2" s="7">
+        <v>2</v>
+      </c>
+      <c r="D2" s="3">
+        <v>3</v>
+      </c>
+      <c r="E2" s="3">
         <v>4</v>
       </c>
       <c r="G2">
@@ -852,19 +854,19 @@
       <c r="I2">
         <v>4</v>
       </c>
-      <c r="J2" s="3">
-        <v>4</v>
-      </c>
-      <c r="K2" s="3">
+      <c r="J2" s="2">
+        <v>4</v>
+      </c>
+      <c r="K2" s="2">
         <v>4</v>
       </c>
       <c r="O2" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="U2">
-        <v>3</v>
-      </c>
-      <c r="X2">
+      <c r="W2">
+        <v>3</v>
+      </c>
+      <c r="Z2">
         <v>5</v>
       </c>
     </row>
@@ -872,13 +874,13 @@
       <c r="A3" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="8">
-        <v>2</v>
-      </c>
-      <c r="D3" s="4">
-        <v>3</v>
-      </c>
-      <c r="E3" s="4">
+      <c r="C3" s="7">
+        <v>2</v>
+      </c>
+      <c r="D3" s="3">
+        <v>3</v>
+      </c>
+      <c r="E3" s="3">
         <v>4</v>
       </c>
       <c r="G3">
@@ -890,16 +892,16 @@
       <c r="I3">
         <v>4</v>
       </c>
-      <c r="J3" s="3">
-        <v>4</v>
-      </c>
-      <c r="K3" s="3">
+      <c r="J3" s="2">
+        <v>4</v>
+      </c>
+      <c r="K3" s="2">
         <v>4</v>
       </c>
       <c r="O3" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="U3">
+      <c r="W3">
         <v>6</v>
       </c>
     </row>
@@ -907,13 +909,13 @@
       <c r="A4" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="4">
-        <v>2</v>
-      </c>
-      <c r="D4" s="4">
-        <v>3</v>
-      </c>
-      <c r="E4" s="4">
+      <c r="C4" s="3">
+        <v>2</v>
+      </c>
+      <c r="D4" s="3">
+        <v>3</v>
+      </c>
+      <c r="E4" s="3">
         <v>4</v>
       </c>
       <c r="G4">
@@ -925,10 +927,10 @@
       <c r="I4">
         <v>4</v>
       </c>
-      <c r="J4" s="3">
-        <v>4</v>
-      </c>
-      <c r="K4" s="3">
+      <c r="J4" s="2">
+        <v>4</v>
+      </c>
+      <c r="K4" s="2">
         <v>4</v>
       </c>
       <c r="O4" s="1" t="s">
@@ -942,13 +944,13 @@
       <c r="A5" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="4">
-        <v>2</v>
-      </c>
-      <c r="D5" s="4">
-        <v>3</v>
-      </c>
-      <c r="E5" s="4">
+      <c r="C5" s="3">
+        <v>2</v>
+      </c>
+      <c r="D5" s="3">
+        <v>3</v>
+      </c>
+      <c r="E5" s="3">
         <v>4</v>
       </c>
       <c r="G5">
@@ -960,10 +962,10 @@
       <c r="I5">
         <v>4</v>
       </c>
-      <c r="J5" s="3">
-        <v>4</v>
-      </c>
-      <c r="K5" s="3">
+      <c r="J5" s="2">
+        <v>4</v>
+      </c>
+      <c r="K5" s="2">
         <v>4</v>
       </c>
       <c r="O5" s="1" t="s">
@@ -977,13 +979,13 @@
       <c r="A6" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="4">
-        <v>2</v>
-      </c>
-      <c r="D6" s="4">
-        <v>3</v>
-      </c>
-      <c r="E6" s="4">
+      <c r="C6" s="3">
+        <v>2</v>
+      </c>
+      <c r="D6" s="3">
+        <v>3</v>
+      </c>
+      <c r="E6" s="3">
         <v>4</v>
       </c>
       <c r="G6">
@@ -995,10 +997,10 @@
       <c r="I6">
         <v>4</v>
       </c>
-      <c r="J6" s="3">
-        <v>4</v>
-      </c>
-      <c r="K6" s="3">
+      <c r="J6" s="2">
+        <v>4</v>
+      </c>
+      <c r="K6" s="2">
         <v>4</v>
       </c>
     </row>
@@ -1006,7 +1008,7 @@
       <c r="O7" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="P7" s="4">
+      <c r="P7" s="3">
         <v>2</v>
       </c>
     </row>
@@ -1026,13 +1028,13 @@
       <c r="I8">
         <v>6</v>
       </c>
-      <c r="J8" s="3">
+      <c r="J8" s="2">
         <v>7</v>
       </c>
       <c r="O8" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="P8" s="4">
+      <c r="P8" s="3">
         <v>2</v>
       </c>
     </row>
@@ -1052,13 +1054,13 @@
       <c r="I9">
         <v>6</v>
       </c>
-      <c r="J9" s="3">
+      <c r="J9" s="2">
         <v>7</v>
       </c>
       <c r="O9" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="P9" s="4">
+      <c r="P9" s="3">
         <v>2</v>
       </c>
     </row>
@@ -1078,13 +1080,13 @@
       <c r="I10">
         <v>6</v>
       </c>
-      <c r="J10" s="3">
+      <c r="J10" s="2">
         <v>7</v>
       </c>
       <c r="O10" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="P10" s="4">
+      <c r="P10" s="3">
         <v>2</v>
       </c>
     </row>
@@ -1104,13 +1106,13 @@
       <c r="I11">
         <v>6</v>
       </c>
-      <c r="J11" s="3">
+      <c r="J11" s="2">
         <v>7</v>
       </c>
       <c r="O11" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="P11" s="4">
+      <c r="P11" s="3">
         <v>2</v>
       </c>
     </row>
@@ -1118,7 +1120,7 @@
       <c r="O12" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="P12" s="4">
+      <c r="P12" s="3">
         <v>2</v>
       </c>
     </row>
@@ -1135,13 +1137,13 @@
       <c r="I13">
         <v>6</v>
       </c>
-      <c r="J13" s="3">
+      <c r="J13" s="2">
         <v>7</v>
       </c>
       <c r="O13" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="P13" s="4">
+      <c r="P13" s="3">
         <v>2</v>
       </c>
     </row>
@@ -1163,7 +1165,7 @@
       <c r="O15" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="P15" s="4">
+      <c r="P15" s="3">
         <v>2</v>
       </c>
     </row>
@@ -1180,13 +1182,13 @@
       <c r="I16">
         <v>6</v>
       </c>
-      <c r="J16" s="3">
+      <c r="J16" s="2">
         <v>7</v>
       </c>
       <c r="O16" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="P16" s="4">
+      <c r="P16" s="3">
         <v>2</v>
       </c>
     </row>
@@ -1200,7 +1202,7 @@
       <c r="O17" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="P17" s="4">
+      <c r="P17" s="3">
         <v>2</v>
       </c>
     </row>
@@ -1214,7 +1216,7 @@
       <c r="O18" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="P18" s="4">
+      <c r="P18" s="3">
         <v>2</v>
       </c>
     </row>
@@ -1222,7 +1224,7 @@
       <c r="O19" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="P19" s="4">
+      <c r="P19" s="3">
         <v>2</v>
       </c>
     </row>
@@ -1239,7 +1241,7 @@
       <c r="O20" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="P20" s="4">
+      <c r="P20" s="3">
         <v>2</v>
       </c>
     </row>
@@ -1265,10 +1267,10 @@
       <c r="I21">
         <v>4</v>
       </c>
-      <c r="J21" s="3">
-        <v>4</v>
-      </c>
-      <c r="K21" s="3">
+      <c r="J21" s="2">
+        <v>4</v>
+      </c>
+      <c r="K21" s="2">
         <v>4</v>
       </c>
     </row>
@@ -1288,29 +1290,29 @@
       <c r="O22" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="Q22" s="4">
-        <v>2</v>
-      </c>
-      <c r="R22" s="4">
-        <v>3</v>
-      </c>
-      <c r="S22" s="4">
-        <v>4</v>
-      </c>
-      <c r="U22" s="4">
-        <v>4</v>
-      </c>
-      <c r="V22" s="5">
-        <v>4</v>
-      </c>
-      <c r="W22" s="5">
+      <c r="Q22" s="3">
+        <v>2</v>
+      </c>
+      <c r="R22" s="3">
+        <v>3</v>
+      </c>
+      <c r="S22" s="3">
+        <v>4</v>
+      </c>
+      <c r="U22" s="3">
+        <v>6</v>
+      </c>
+      <c r="V22" s="4">
+        <v>5</v>
+      </c>
+      <c r="W22" s="3">
+        <v>4</v>
+      </c>
+      <c r="X22" s="4">
         <v>4</v>
       </c>
       <c r="Y22" s="4">
-        <v>6</v>
-      </c>
-      <c r="Z22" s="5">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="23" spans="1:26" x14ac:dyDescent="0.25">
@@ -1329,19 +1331,19 @@
       <c r="O23" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="Q23" s="4">
-        <v>2</v>
-      </c>
-      <c r="R23" s="4">
-        <v>3</v>
-      </c>
-      <c r="T23" s="4">
-        <v>4</v>
-      </c>
-      <c r="U23" s="4">
-        <v>4</v>
-      </c>
-      <c r="W23" s="5">
+      <c r="Q23" s="3">
+        <v>2</v>
+      </c>
+      <c r="R23" s="3">
+        <v>3</v>
+      </c>
+      <c r="T23" s="3">
+        <v>4</v>
+      </c>
+      <c r="W23" s="3">
+        <v>4</v>
+      </c>
+      <c r="Y23" s="4">
         <v>4</v>
       </c>
     </row>
@@ -1349,19 +1351,19 @@
       <c r="O24" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="Q24" s="4">
-        <v>2</v>
-      </c>
-      <c r="R24" s="4">
-        <v>3</v>
-      </c>
-      <c r="S24" s="4">
-        <v>4</v>
-      </c>
-      <c r="U24" s="4">
-        <v>4</v>
-      </c>
-      <c r="V24" s="5">
+      <c r="Q24" s="3">
+        <v>2</v>
+      </c>
+      <c r="R24" s="3">
+        <v>3</v>
+      </c>
+      <c r="S24" s="3">
+        <v>4</v>
+      </c>
+      <c r="W24" s="3">
+        <v>4</v>
+      </c>
+      <c r="X24" s="4">
         <v>4</v>
       </c>
     </row>
@@ -1369,52 +1371,52 @@
       <c r="A25" t="s">
         <v>23</v>
       </c>
-      <c r="M25" s="3">
+      <c r="M25" s="2">
         <v>2</v>
       </c>
       <c r="O25" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="R25" s="4">
-        <v>3</v>
-      </c>
-      <c r="S25" s="4">
-        <v>4</v>
-      </c>
-      <c r="U25" s="4">
-        <v>4</v>
-      </c>
-      <c r="V25" s="7">
-        <v>5</v>
-      </c>
-      <c r="W25" s="7">
-        <v>5</v>
-      </c>
-      <c r="X25" s="6"/>
-      <c r="Y25" s="7">
-        <v>6</v>
-      </c>
-      <c r="Z25" s="7">
-        <v>6</v>
-      </c>
+      <c r="R25" s="3">
+        <v>3</v>
+      </c>
+      <c r="S25" s="3">
+        <v>4</v>
+      </c>
+      <c r="U25" s="6">
+        <v>6</v>
+      </c>
+      <c r="V25" s="6">
+        <v>6</v>
+      </c>
+      <c r="W25" s="3">
+        <v>4</v>
+      </c>
+      <c r="X25" s="6">
+        <v>5</v>
+      </c>
+      <c r="Y25" s="6">
+        <v>5</v>
+      </c>
+      <c r="Z25" s="5"/>
     </row>
     <row r="26" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>24</v>
       </c>
-      <c r="M26" s="3">
+      <c r="M26" s="2">
         <v>2</v>
       </c>
       <c r="O26" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="R26" s="4">
-        <v>3</v>
-      </c>
-      <c r="T26" s="4">
-        <v>4</v>
-      </c>
-      <c r="U26" s="4">
+      <c r="R26" s="3">
+        <v>3</v>
+      </c>
+      <c r="T26" s="3">
+        <v>4</v>
+      </c>
+      <c r="W26" s="3">
         <v>4</v>
       </c>
     </row>
@@ -1422,19 +1424,19 @@
       <c r="A27" t="s">
         <v>25</v>
       </c>
-      <c r="M27" s="3">
+      <c r="M27" s="2">
         <v>2</v>
       </c>
       <c r="O27" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="R27" s="4">
-        <v>3</v>
-      </c>
-      <c r="S27" s="4">
-        <v>4</v>
-      </c>
-      <c r="U27" s="4">
+      <c r="R27" s="3">
+        <v>3</v>
+      </c>
+      <c r="S27" s="3">
+        <v>4</v>
+      </c>
+      <c r="W27" s="3">
         <v>4</v>
       </c>
     </row>
@@ -1442,7 +1444,7 @@
       <c r="A28" t="s">
         <v>26</v>
       </c>
-      <c r="M28" s="3">
+      <c r="M28" s="2">
         <v>2</v>
       </c>
     </row>
@@ -1450,7 +1452,7 @@
       <c r="A29" t="s">
         <v>27</v>
       </c>
-      <c r="M29" s="3">
+      <c r="M29" s="2">
         <v>2</v>
       </c>
       <c r="O29" s="1" t="s">
@@ -1464,7 +1466,7 @@
       <c r="A30" t="s">
         <v>28</v>
       </c>
-      <c r="M30" s="3">
+      <c r="M30" s="2">
         <v>2</v>
       </c>
       <c r="O30" s="1" t="s">
@@ -1478,7 +1480,7 @@
       <c r="A31" t="s">
         <v>29</v>
       </c>
-      <c r="M31" s="3">
+      <c r="M31" s="2">
         <v>2</v>
       </c>
       <c r="O31" s="1" t="s">
@@ -1492,7 +1494,7 @@
       <c r="A32" t="s">
         <v>30</v>
       </c>
-      <c r="M32" s="3">
+      <c r="M32" s="2">
         <v>2</v>
       </c>
       <c r="O32" s="1" t="s">
@@ -1506,7 +1508,7 @@
       <c r="O34" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="P34" s="4">
+      <c r="P34" s="3">
         <v>7</v>
       </c>
     </row>
@@ -1514,7 +1516,7 @@
       <c r="O35" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="P35" s="4">
+      <c r="P35" s="3">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Revert, use LDA microcode branch to implement ORA, AND, EOR, ADC, SBC
</commit_message>
<xml_diff>
--- a/cpu/opcodes.xlsx
+++ b/cpu/opcodes.xlsx
@@ -845,19 +845,19 @@
       <c r="E2" s="3">
         <v>4</v>
       </c>
-      <c r="G2">
-        <v>6</v>
-      </c>
-      <c r="H2">
-        <v>5</v>
-      </c>
-      <c r="I2">
-        <v>4</v>
-      </c>
-      <c r="J2" s="2">
-        <v>4</v>
-      </c>
-      <c r="K2" s="2">
+      <c r="G2" s="3">
+        <v>6</v>
+      </c>
+      <c r="H2" s="4">
+        <v>5</v>
+      </c>
+      <c r="I2" s="3">
+        <v>4</v>
+      </c>
+      <c r="J2" s="4">
+        <v>4</v>
+      </c>
+      <c r="K2" s="4">
         <v>4</v>
       </c>
       <c r="O2" s="1" t="s">
@@ -883,19 +883,19 @@
       <c r="E3" s="3">
         <v>4</v>
       </c>
-      <c r="G3">
-        <v>6</v>
-      </c>
-      <c r="H3">
-        <v>5</v>
-      </c>
-      <c r="I3">
-        <v>4</v>
-      </c>
-      <c r="J3" s="2">
-        <v>4</v>
-      </c>
-      <c r="K3" s="2">
+      <c r="G3" s="3">
+        <v>6</v>
+      </c>
+      <c r="H3" s="4">
+        <v>5</v>
+      </c>
+      <c r="I3" s="3">
+        <v>4</v>
+      </c>
+      <c r="J3" s="4">
+        <v>4</v>
+      </c>
+      <c r="K3" s="4">
         <v>4</v>
       </c>
       <c r="O3" s="1" t="s">
@@ -918,19 +918,19 @@
       <c r="E4" s="3">
         <v>4</v>
       </c>
-      <c r="G4">
-        <v>6</v>
-      </c>
-      <c r="H4">
-        <v>5</v>
-      </c>
-      <c r="I4">
-        <v>4</v>
-      </c>
-      <c r="J4" s="2">
-        <v>4</v>
-      </c>
-      <c r="K4" s="2">
+      <c r="G4" s="3">
+        <v>6</v>
+      </c>
+      <c r="H4" s="4">
+        <v>5</v>
+      </c>
+      <c r="I4" s="3">
+        <v>4</v>
+      </c>
+      <c r="J4" s="4">
+        <v>4</v>
+      </c>
+      <c r="K4" s="4">
         <v>4</v>
       </c>
       <c r="O4" s="1" t="s">
@@ -953,19 +953,19 @@
       <c r="E5" s="3">
         <v>4</v>
       </c>
-      <c r="G5">
-        <v>6</v>
-      </c>
-      <c r="H5">
-        <v>5</v>
-      </c>
-      <c r="I5">
-        <v>4</v>
-      </c>
-      <c r="J5" s="2">
-        <v>4</v>
-      </c>
-      <c r="K5" s="2">
+      <c r="G5" s="3">
+        <v>6</v>
+      </c>
+      <c r="H5" s="4">
+        <v>5</v>
+      </c>
+      <c r="I5" s="3">
+        <v>4</v>
+      </c>
+      <c r="J5" s="4">
+        <v>4</v>
+      </c>
+      <c r="K5" s="4">
         <v>4</v>
       </c>
       <c r="O5" s="1" t="s">
@@ -988,19 +988,19 @@
       <c r="E6" s="3">
         <v>4</v>
       </c>
-      <c r="G6">
-        <v>6</v>
-      </c>
-      <c r="H6">
-        <v>5</v>
-      </c>
-      <c r="I6">
-        <v>4</v>
-      </c>
-      <c r="J6" s="2">
-        <v>4</v>
-      </c>
-      <c r="K6" s="2">
+      <c r="G6" s="3">
+        <v>6</v>
+      </c>
+      <c r="H6" s="4">
+        <v>5</v>
+      </c>
+      <c r="I6" s="3">
+        <v>4</v>
+      </c>
+      <c r="J6" s="4">
+        <v>4</v>
+      </c>
+      <c r="K6" s="4">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
DEX, DEY, INX, INY
</commit_message>
<xml_diff>
--- a/cpu/opcodes.xlsx
+++ b/cpu/opcodes.xlsx
@@ -1151,7 +1151,7 @@
       <c r="A14" t="s">
         <v>14</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="3">
         <v>2</v>
       </c>
     </row>
@@ -1159,7 +1159,7 @@
       <c r="A15" t="s">
         <v>15</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="3">
         <v>2</v>
       </c>
       <c r="O15" s="1" t="s">
@@ -1196,7 +1196,7 @@
       <c r="A17" t="s">
         <v>17</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="3">
         <v>2</v>
       </c>
       <c r="O17" s="1" t="s">
@@ -1210,7 +1210,7 @@
       <c r="A18" t="s">
         <v>18</v>
       </c>
-      <c r="B18">
+      <c r="B18" s="3">
         <v>2</v>
       </c>
       <c r="O18" s="1" t="s">

</xml_diff>

<commit_message>
DEC d; DEC d, x
</commit_message>
<xml_diff>
--- a/cpu/opcodes.xlsx
+++ b/cpu/opcodes.xlsx
@@ -1173,10 +1173,10 @@
       <c r="A16" t="s">
         <v>16</v>
       </c>
-      <c r="D16">
-        <v>5</v>
-      </c>
-      <c r="E16">
+      <c r="D16" s="3">
+        <v>5</v>
+      </c>
+      <c r="E16" s="3">
         <v>6</v>
       </c>
       <c r="I16">

</xml_diff>

<commit_message>
DEC a; DEC a, x
</commit_message>
<xml_diff>
--- a/cpu/opcodes.xlsx
+++ b/cpu/opcodes.xlsx
@@ -1179,10 +1179,10 @@
       <c r="E16" s="3">
         <v>6</v>
       </c>
-      <c r="I16">
-        <v>6</v>
-      </c>
-      <c r="J16" s="2">
+      <c r="I16" s="3">
+        <v>6</v>
+      </c>
+      <c r="J16" s="4">
         <v>7</v>
       </c>
       <c r="O16" s="1" t="s">

</xml_diff>

<commit_message>
ASL; ROL; LSR; ROR
</commit_message>
<xml_diff>
--- a/cpu/opcodes.xlsx
+++ b/cpu/opcodes.xlsx
@@ -1016,19 +1016,19 @@
       <c r="A8" t="s">
         <v>9</v>
       </c>
-      <c r="B8">
-        <v>2</v>
-      </c>
-      <c r="D8">
-        <v>5</v>
-      </c>
-      <c r="E8">
-        <v>6</v>
-      </c>
-      <c r="I8">
-        <v>6</v>
-      </c>
-      <c r="J8" s="2">
+      <c r="B8" s="3">
+        <v>2</v>
+      </c>
+      <c r="D8" s="3">
+        <v>5</v>
+      </c>
+      <c r="E8" s="3">
+        <v>6</v>
+      </c>
+      <c r="I8" s="3">
+        <v>6</v>
+      </c>
+      <c r="J8" s="4">
         <v>7</v>
       </c>
       <c r="O8" s="1" t="s">
@@ -1042,19 +1042,19 @@
       <c r="A9" t="s">
         <v>10</v>
       </c>
-      <c r="B9">
-        <v>2</v>
-      </c>
-      <c r="D9">
-        <v>5</v>
-      </c>
-      <c r="E9">
-        <v>6</v>
-      </c>
-      <c r="I9">
-        <v>6</v>
-      </c>
-      <c r="J9" s="2">
+      <c r="B9" s="3">
+        <v>2</v>
+      </c>
+      <c r="D9" s="3">
+        <v>5</v>
+      </c>
+      <c r="E9" s="3">
+        <v>6</v>
+      </c>
+      <c r="I9" s="3">
+        <v>6</v>
+      </c>
+      <c r="J9" s="4">
         <v>7</v>
       </c>
       <c r="O9" s="1" t="s">
@@ -1068,19 +1068,19 @@
       <c r="A10" t="s">
         <v>11</v>
       </c>
-      <c r="B10">
-        <v>2</v>
-      </c>
-      <c r="D10">
-        <v>5</v>
-      </c>
-      <c r="E10">
-        <v>6</v>
-      </c>
-      <c r="I10">
-        <v>6</v>
-      </c>
-      <c r="J10" s="2">
+      <c r="B10" s="3">
+        <v>2</v>
+      </c>
+      <c r="D10" s="3">
+        <v>5</v>
+      </c>
+      <c r="E10" s="3">
+        <v>6</v>
+      </c>
+      <c r="I10" s="3">
+        <v>6</v>
+      </c>
+      <c r="J10" s="4">
         <v>7</v>
       </c>
       <c r="O10" s="1" t="s">
@@ -1094,19 +1094,19 @@
       <c r="A11" t="s">
         <v>12</v>
       </c>
-      <c r="B11">
-        <v>2</v>
-      </c>
-      <c r="D11">
-        <v>5</v>
-      </c>
-      <c r="E11">
-        <v>6</v>
-      </c>
-      <c r="I11">
-        <v>6</v>
-      </c>
-      <c r="J11" s="2">
+      <c r="B11" s="3">
+        <v>2</v>
+      </c>
+      <c r="D11" s="3">
+        <v>5</v>
+      </c>
+      <c r="E11" s="3">
+        <v>6</v>
+      </c>
+      <c r="I11" s="3">
+        <v>6</v>
+      </c>
+      <c r="J11" s="4">
         <v>7</v>
       </c>
       <c r="O11" s="1" t="s">

</xml_diff>

<commit_message>
BIT; CMP; CPX; CPY
</commit_message>
<xml_diff>
--- a/cpu/opcodes.xlsx
+++ b/cpu/opcodes.xlsx
@@ -1232,10 +1232,10 @@
       <c r="A20" t="s">
         <v>19</v>
       </c>
-      <c r="D20">
-        <v>3</v>
-      </c>
-      <c r="I20">
+      <c r="D20" s="3">
+        <v>3</v>
+      </c>
+      <c r="I20" s="3">
         <v>4</v>
       </c>
       <c r="O20" s="1" t="s">
@@ -1249,28 +1249,28 @@
       <c r="A21" t="s">
         <v>20</v>
       </c>
-      <c r="C21">
-        <v>2</v>
-      </c>
-      <c r="D21">
-        <v>3</v>
-      </c>
-      <c r="E21">
-        <v>4</v>
-      </c>
-      <c r="G21">
-        <v>6</v>
-      </c>
-      <c r="H21">
-        <v>5</v>
-      </c>
-      <c r="I21">
-        <v>4</v>
-      </c>
-      <c r="J21" s="2">
-        <v>4</v>
-      </c>
-      <c r="K21" s="2">
+      <c r="C21" s="3">
+        <v>2</v>
+      </c>
+      <c r="D21" s="3">
+        <v>3</v>
+      </c>
+      <c r="E21" s="3">
+        <v>4</v>
+      </c>
+      <c r="G21" s="3">
+        <v>6</v>
+      </c>
+      <c r="H21" s="3">
+        <v>5</v>
+      </c>
+      <c r="I21" s="3">
+        <v>4</v>
+      </c>
+      <c r="J21" s="4">
+        <v>4</v>
+      </c>
+      <c r="K21" s="4">
         <v>4</v>
       </c>
     </row>
@@ -1278,13 +1278,13 @@
       <c r="A22" t="s">
         <v>21</v>
       </c>
-      <c r="C22">
-        <v>2</v>
-      </c>
-      <c r="D22">
-        <v>3</v>
-      </c>
-      <c r="I22">
+      <c r="C22" s="3">
+        <v>2</v>
+      </c>
+      <c r="D22" s="3">
+        <v>3</v>
+      </c>
+      <c r="I22" s="3">
         <v>4</v>
       </c>
       <c r="O22" s="1" t="s">
@@ -1319,13 +1319,13 @@
       <c r="A23" t="s">
         <v>22</v>
       </c>
-      <c r="C23">
-        <v>2</v>
-      </c>
-      <c r="D23">
-        <v>3</v>
-      </c>
-      <c r="I23">
+      <c r="C23" s="3">
+        <v>2</v>
+      </c>
+      <c r="D23" s="3">
+        <v>3</v>
+      </c>
+      <c r="I23" s="3">
         <v>4</v>
       </c>
       <c r="O23" s="1" t="s">

</xml_diff>

<commit_message>
PLA; PHA; PLP; PHP
</commit_message>
<xml_diff>
--- a/cpu/opcodes.xlsx
+++ b/cpu/opcodes.xlsx
@@ -1458,7 +1458,7 @@
       <c r="O29" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="P29">
+      <c r="P29" s="3">
         <v>3</v>
       </c>
     </row>
@@ -1472,7 +1472,7 @@
       <c r="O30" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="P30">
+      <c r="P30" s="3">
         <v>3</v>
       </c>
     </row>
@@ -1486,7 +1486,7 @@
       <c r="O31" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="P31">
+      <c r="P31" s="3">
         <v>4</v>
       </c>
     </row>
@@ -1500,7 +1500,7 @@
       <c r="O32" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="P32">
+      <c r="P32" s="3">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
JMP a; JMP (a)
</commit_message>
<xml_diff>
--- a/cpu/opcodes.xlsx
+++ b/cpu/opcodes.xlsx
@@ -863,10 +863,10 @@
       <c r="O2" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="W2">
-        <v>3</v>
-      </c>
-      <c r="Z2">
+      <c r="W2" s="3">
+        <v>3</v>
+      </c>
+      <c r="Z2" s="3">
         <v>5</v>
       </c>
     </row>

</xml_diff>